<commit_message>
Add /start-survey ajax call
</commit_message>
<xml_diff>
--- a/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
+++ b/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalija\Desktop\surveyapp\surveyapp\data\users_surveys\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B201FF7-4CF3-4BFE-A4F4-1AC46E756812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>conversation</t>
   </si>
@@ -44,13 +50,16 @@
   </si>
   <si>
     <t>conv_4</t>
+  </si>
+  <si>
+    <t>2023-07-10T11:55:56.998Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +122,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +174,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,6 +208,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,9 +243,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,14 +419,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="26.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,27 +448,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Finish /start-survey call, work with timestamps in .js and .py
</commit_message>
<xml_diff>
--- a/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
+++ b/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalija\Desktop\surveyapp\surveyapp\data\users_surveys\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B201FF7-4CF3-4BFE-A4F4-1AC46E756812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>conversation</t>
   </si>
@@ -50,16 +44,13 @@
   </si>
   <si>
     <t>conv_4</t>
-  </si>
-  <si>
-    <t>2023-07-10T11:55:56.998Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,21 +113,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -174,7 +157,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -208,7 +191,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -243,10 +225,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -419,19 +400,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="26.36328125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,30 +424,33 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>1689002548051</v>
+      </c>
+      <c r="C2">
+        <v>1689002848051</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Finish /give-reason call, coundown fix, reason end_time fix
</commit_message>
<xml_diff>
--- a/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
+++ b/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>conversation</t>
   </si>
@@ -46,7 +46,19 @@
     <t>conv_4</t>
   </si>
   <si>
-    <t>3</t>
+    <t>haha idk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lepo </t>
+  </si>
+  <si>
+    <t>sdgefc</t>
+  </si>
+  <si>
+    <t>xsefzw</t>
+  </si>
+  <si>
+    <t>sadaws</t>
   </si>
 </sst>
 </file>
@@ -437,7 +449,7 @@
       <c r="C2">
         <v>1689005004649</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -445,20 +457,68 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
+      <c r="B3">
+        <v>1689015608877</v>
+      </c>
+      <c r="C3">
+        <v>1689015613411</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
+      <c r="B4">
+        <v>1689015617819</v>
+      </c>
+      <c r="C4">
+        <v>1689015626587</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
+      <c r="B5">
+        <v>1689015629330</v>
+      </c>
+      <c r="C5">
+        <v>1689015710625</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
+      </c>
+      <c r="B6">
+        <v>1689015713255</v>
+      </c>
+      <c r="C6">
+        <v>1689015730798</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Countdown timer fix, add /reset-survey
</commit_message>
<xml_diff>
--- a/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
+++ b/surveyapp/data/users_surveys/iwjCyatX7NJI65FnA8wjQMaBx3u8QKF9PGywJWiw-dw.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>conversation</t>
   </si>
@@ -44,21 +44,6 @@
   </si>
   <si>
     <t>conv_4</t>
-  </si>
-  <si>
-    <t>haha idk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lepo </t>
-  </si>
-  <si>
-    <t>sdgefc</t>
-  </si>
-  <si>
-    <t>xsefzw</t>
-  </si>
-  <si>
-    <t>sdew</t>
   </si>
 </sst>
 </file>
@@ -443,82 +428,25 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1689004911977</v>
-      </c>
-      <c r="C2">
-        <v>1689005004649</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>1689015608877</v>
-      </c>
-      <c r="C3">
-        <v>1689015613411</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>1689015617819</v>
-      </c>
-      <c r="C4">
-        <v>1689015626587</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1689015629330</v>
-      </c>
-      <c r="C5">
-        <v>1689015710625</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6">
-        <v>1689015713255</v>
-      </c>
-      <c r="C6">
-        <v>1689015730798</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>